<commit_message>
Tableau de synthèse complet
</commit_message>
<xml_diff>
--- a/Integration_Templates/PDF/GARRIGUES_Jean_Tableau_de_synthèse_Epreuve_E4_BTS_SIO_2023.xlsx
+++ b/Integration_Templates/PDF/GARRIGUES_Jean_Tableau_de_synthèse_Epreuve_E4_BTS_SIO_2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean2\Documents\Devoirs\BTS_SIO_2\Portfolio\barbaredunord.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean2\Documents\Devoirs\BTS_SIO_2\Portfolio\barbaredunord.github.io\Integration_Templates\PDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B50579-C16E-49F0-9580-EE495CC5F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B503BCD-3EB7-4D77-8CAE-9A99CB98317E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>09/01/2023 - 17/02/2023</t>
   </si>
   <si>
-    <t>N° candidat : 0714</t>
-  </si>
-  <si>
     <t>NOM et prénom : GARRIGUES Jean</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Portfolio sur GitHub Pages</t>
+  </si>
+  <si>
+    <t>N° candidat : 071405406HH</t>
   </si>
 </sst>
 </file>
@@ -169,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -244,6 +244,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -709,9 +716,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="17" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -721,9 +725,66 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -748,61 +809,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1149,8 +1156,8 @@
   </sheetPr>
   <dimension ref="A1:AQ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1163,83 +1170,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:43" ht="40.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="29" t="s">
+      <c r="A3" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="48"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="49" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="A5" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="36" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1262,24 +1269,24 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1319,16 +1326,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1369,13 +1376,13 @@
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>44501</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="45"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
       <c r="I9"/>
@@ -1418,13 +1425,13 @@
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
       <c r="I10"/>
@@ -1470,10 +1477,10 @@
       <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="44"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
       <c r="I11"/>
@@ -1519,10 +1526,10 @@
       <c r="B12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="45"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="44"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
       <c r="I12"/>
@@ -1563,13 +1570,13 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="14"/>
-      <c r="D13" s="45"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1611,16 +1618,16 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1664,12 +1671,12 @@
       <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="47"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="48"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="25"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1977,16 +1984,16 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2030,12 +2037,12 @@
       <c r="B23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="49"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="48"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="25"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2435,6 +2442,11 @@
     <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2442,11 +2454,6 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>